<commit_message>
removed POP EDA from WEIGHTS tab
</commit_message>
<xml_diff>
--- a/input/community_cohort_inputs_2022.xlsx
+++ b/input/community_cohort_inputs_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npeterson\Documents\GitHub\community-cohort-tool\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amcadams\GitHub\community-cohort-tool\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36DDCD9-BD5F-4C42-986E-5A8F34BED458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C96A058-2EA7-4E75-956E-B49074CCF310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9165" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FACTORS_MUNI" sheetId="1" r:id="rId1"/>
@@ -2507,7 +2507,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2523,17 +2523,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -2584,21 +2583,21 @@
   <dxfs count="2">
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF800000"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2896,7 +2895,7 @@
     <col min="4" max="4" width="12.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" style="26" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="8" bestFit="1" customWidth="1"/>
@@ -2910,22 +2909,22 @@
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="25" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="6" t="s">
@@ -2963,7 +2962,7 @@
       <c r="G2" s="9">
         <v>0.5683715198028122</v>
       </c>
-      <c r="H2" s="27">
+      <c r="H2" s="26">
         <f t="shared" ref="H2:H65" si="0">E2+F2</f>
         <v>2380675531</v>
       </c>
@@ -3006,7 +3005,7 @@
       <c r="G3" s="9">
         <v>4.4444444444444446E-2</v>
       </c>
-      <c r="H3" s="27">
+      <c r="H3" s="26">
         <f t="shared" si="0"/>
         <v>1741509913</v>
       </c>
@@ -3049,7 +3048,7 @@
       <c r="G4" s="9">
         <v>2.2556785395792898E-2</v>
       </c>
-      <c r="H4" s="27">
+      <c r="H4" s="26">
         <f t="shared" si="0"/>
         <v>945954610</v>
       </c>
@@ -3092,7 +3091,7 @@
       <c r="G5" s="9">
         <v>0</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5" s="26">
         <f t="shared" si="0"/>
         <v>767561288</v>
       </c>
@@ -3135,7 +3134,7 @@
       <c r="G6" s="9">
         <v>0.17019413976002884</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="26">
         <f t="shared" si="0"/>
         <v>4650836168</v>
       </c>
@@ -3178,7 +3177,7 @@
       <c r="G7" s="9">
         <v>0.62980359140809339</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="26">
         <f t="shared" si="0"/>
         <v>6507924621</v>
       </c>
@@ -3221,7 +3220,7 @@
       <c r="G8" s="9">
         <v>0</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="26">
         <f t="shared" si="0"/>
         <v>307654648</v>
       </c>
@@ -3264,7 +3263,7 @@
       <c r="G9" s="9">
         <v>0</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="26">
         <f t="shared" si="0"/>
         <v>1291087494</v>
       </c>
@@ -3307,7 +3306,7 @@
       <c r="G10" s="9">
         <v>3.0384054448225572E-2</v>
       </c>
-      <c r="H10" s="27">
+      <c r="H10" s="26">
         <f t="shared" si="0"/>
         <v>457012410</v>
       </c>
@@ -3350,7 +3349,7 @@
       <c r="G11" s="9">
         <v>0.18829826055224425</v>
       </c>
-      <c r="H11" s="27">
+      <c r="H11" s="26">
         <f t="shared" si="0"/>
         <v>1417628523</v>
       </c>
@@ -3393,7 +3392,7 @@
       <c r="G12" s="9">
         <v>0</v>
       </c>
-      <c r="H12" s="27">
+      <c r="H12" s="26">
         <f t="shared" si="0"/>
         <v>1546844056</v>
       </c>
@@ -3436,7 +3435,7 @@
       <c r="G13" s="9">
         <v>9.1725735139308026E-2</v>
       </c>
-      <c r="H13" s="27">
+      <c r="H13" s="26">
         <f t="shared" si="0"/>
         <v>289323245</v>
       </c>
@@ -3479,7 +3478,7 @@
       <c r="G14" s="9">
         <v>2.3255813953488372E-2</v>
       </c>
-      <c r="H14" s="27">
+      <c r="H14" s="26">
         <f t="shared" si="0"/>
         <v>868551620</v>
       </c>
@@ -3522,7 +3521,7 @@
       <c r="G15" s="9">
         <v>0</v>
       </c>
-      <c r="H15" s="27">
+      <c r="H15" s="26">
         <f t="shared" si="0"/>
         <v>150464439</v>
       </c>
@@ -3565,7 +3564,7 @@
       <c r="G16" s="9">
         <v>0.83186971100111773</v>
       </c>
-      <c r="H16" s="27">
+      <c r="H16" s="26">
         <f t="shared" si="0"/>
         <v>290761486</v>
       </c>
@@ -3608,7 +3607,7 @@
       <c r="G17" s="9">
         <v>0.25663105299526923</v>
       </c>
-      <c r="H17" s="27">
+      <c r="H17" s="26">
         <f t="shared" si="0"/>
         <v>1259032365</v>
       </c>
@@ -3651,7 +3650,7 @@
       <c r="G18" s="9">
         <v>0</v>
       </c>
-      <c r="H18" s="27">
+      <c r="H18" s="26">
         <f t="shared" si="0"/>
         <v>118820555</v>
       </c>
@@ -3694,7 +3693,7 @@
       <c r="G19" s="9">
         <v>0.72496069868995638</v>
       </c>
-      <c r="H19" s="27">
+      <c r="H19" s="26">
         <f t="shared" si="0"/>
         <v>1135937700</v>
       </c>
@@ -3737,7 +3736,7 @@
       <c r="G20" s="9">
         <v>0</v>
       </c>
-      <c r="H20" s="27">
+      <c r="H20" s="26">
         <f t="shared" si="0"/>
         <v>51900276</v>
       </c>
@@ -3780,7 +3779,7 @@
       <c r="G21" s="9">
         <v>0.12523456348851755</v>
       </c>
-      <c r="H21" s="27">
+      <c r="H21" s="26">
         <f t="shared" si="0"/>
         <v>1701238858</v>
       </c>
@@ -3823,7 +3822,7 @@
       <c r="G22" s="9">
         <v>1</v>
       </c>
-      <c r="H22" s="27">
+      <c r="H22" s="26">
         <f t="shared" si="0"/>
         <v>371919382</v>
       </c>
@@ -3866,7 +3865,7 @@
       <c r="G23" s="9">
         <v>0.25710884445767163</v>
       </c>
-      <c r="H23" s="27">
+      <c r="H23" s="26">
         <f t="shared" si="0"/>
         <v>3851050532</v>
       </c>
@@ -3909,7 +3908,7 @@
       <c r="G24" s="9">
         <v>0</v>
       </c>
-      <c r="H24" s="27">
+      <c r="H24" s="26">
         <f t="shared" si="0"/>
         <v>16410898</v>
       </c>
@@ -3952,7 +3951,7 @@
       <c r="G25" s="9">
         <v>0</v>
       </c>
-      <c r="H25" s="27">
+      <c r="H25" s="26">
         <f t="shared" si="0"/>
         <v>161737997</v>
       </c>
@@ -3995,7 +3994,7 @@
       <c r="G26" s="9">
         <v>0.30275444881658542</v>
       </c>
-      <c r="H26" s="27">
+      <c r="H26" s="26">
         <f t="shared" si="0"/>
         <v>1057887956</v>
       </c>
@@ -4038,7 +4037,7 @@
       <c r="G27" s="9">
         <v>0.67529382345586397</v>
       </c>
-      <c r="H27" s="27">
+      <c r="H27" s="26">
         <f t="shared" si="0"/>
         <v>467722720</v>
       </c>
@@ -4081,7 +4080,7 @@
       <c r="G28" s="9">
         <v>0.7737215033887862</v>
       </c>
-      <c r="H28" s="27">
+      <c r="H28" s="26">
         <f t="shared" si="0"/>
         <v>479569799</v>
       </c>
@@ -4124,7 +4123,7 @@
       <c r="G29" s="9">
         <v>4.30435990002777E-3</v>
       </c>
-      <c r="H29" s="27">
+      <c r="H29" s="26">
         <f t="shared" si="0"/>
         <v>2533412043</v>
       </c>
@@ -4167,7 +4166,7 @@
       <c r="G30" s="9">
         <v>0</v>
       </c>
-      <c r="H30" s="27">
+      <c r="H30" s="26">
         <f t="shared" si="0"/>
         <v>64515889</v>
       </c>
@@ -4210,7 +4209,7 @@
       <c r="G31" s="9">
         <v>0.6628961581575461</v>
       </c>
-      <c r="H31" s="27">
+      <c r="H31" s="26">
         <f t="shared" si="0"/>
         <v>804065191</v>
       </c>
@@ -4253,7 +4252,7 @@
       <c r="G32" s="9">
         <v>0</v>
       </c>
-      <c r="H32" s="27">
+      <c r="H32" s="26">
         <f t="shared" si="0"/>
         <v>22596517</v>
       </c>
@@ -4296,7 +4295,7 @@
       <c r="G33" s="9">
         <v>1</v>
       </c>
-      <c r="H33" s="27">
+      <c r="H33" s="26">
         <f t="shared" si="0"/>
         <v>53093229</v>
       </c>
@@ -4339,7 +4338,7 @@
       <c r="G34" s="9">
         <v>0</v>
       </c>
-      <c r="H34" s="27">
+      <c r="H34" s="26">
         <f t="shared" si="0"/>
         <v>1360308443</v>
       </c>
@@ -4382,7 +4381,7 @@
       <c r="G35" s="9">
         <v>1</v>
       </c>
-      <c r="H35" s="27">
+      <c r="H35" s="26">
         <f t="shared" si="0"/>
         <v>885116808</v>
       </c>
@@ -4425,7 +4424,7 @@
       <c r="G36" s="9">
         <v>0.54448398576512458</v>
       </c>
-      <c r="H36" s="27">
+      <c r="H36" s="26">
         <f t="shared" si="0"/>
         <v>147947495</v>
       </c>
@@ -4468,7 +4467,7 @@
       <c r="G37" s="9">
         <v>0</v>
       </c>
-      <c r="H37" s="27">
+      <c r="H37" s="26">
         <f t="shared" si="0"/>
         <v>506770662</v>
       </c>
@@ -4511,7 +4510,7 @@
       <c r="G38" s="9">
         <v>0.16685903547950018</v>
       </c>
-      <c r="H38" s="27">
+      <c r="H38" s="26">
         <f t="shared" si="0"/>
         <v>2041573836</v>
       </c>
@@ -4554,7 +4553,7 @@
       <c r="G39" s="9">
         <v>0.72645657267725039</v>
       </c>
-      <c r="H39" s="27">
+      <c r="H39" s="26">
         <f t="shared" si="0"/>
         <v>1040628388</v>
       </c>
@@ -4597,7 +4596,7 @@
       <c r="G40" s="9">
         <v>0</v>
       </c>
-      <c r="H40" s="27">
+      <c r="H40" s="26">
         <f t="shared" si="0"/>
         <v>660778336</v>
       </c>
@@ -4640,7 +4639,7 @@
       <c r="G41" s="9">
         <v>0</v>
       </c>
-      <c r="H41" s="27">
+      <c r="H41" s="26">
         <f t="shared" si="0"/>
         <v>505875660</v>
       </c>
@@ -4683,7 +4682,7 @@
       <c r="G42" s="9">
         <v>0.62405129937940307</v>
       </c>
-      <c r="H42" s="27">
+      <c r="H42" s="26">
         <f t="shared" si="0"/>
         <v>118051678598</v>
       </c>
@@ -4726,7 +4725,7 @@
       <c r="G43" s="9">
         <v>0.77678311499272201</v>
       </c>
-      <c r="H43" s="27">
+      <c r="H43" s="26">
         <f t="shared" si="0"/>
         <v>538311518</v>
       </c>
@@ -4769,7 +4768,7 @@
       <c r="G44" s="9">
         <v>0.57756530173907017</v>
       </c>
-      <c r="H44" s="27">
+      <c r="H44" s="26">
         <f t="shared" si="0"/>
         <v>645095122</v>
       </c>
@@ -4812,7 +4811,7 @@
       <c r="G45" s="9">
         <v>1</v>
       </c>
-      <c r="H45" s="27">
+      <c r="H45" s="26">
         <f t="shared" si="0"/>
         <v>1431321666</v>
       </c>
@@ -4855,7 +4854,7 @@
       <c r="G46" s="9">
         <v>0</v>
       </c>
-      <c r="H46" s="27">
+      <c r="H46" s="26">
         <f t="shared" si="0"/>
         <v>681952776</v>
       </c>
@@ -4898,7 +4897,7 @@
       <c r="G47" s="9">
         <v>0</v>
       </c>
-      <c r="H47" s="27">
+      <c r="H47" s="26">
         <f t="shared" si="0"/>
         <v>172485001</v>
       </c>
@@ -4941,7 +4940,7 @@
       <c r="G48" s="9">
         <v>0.43540983606557376</v>
       </c>
-      <c r="H48" s="27">
+      <c r="H48" s="26">
         <f t="shared" si="0"/>
         <v>301635722</v>
       </c>
@@ -4984,7 +4983,7 @@
       <c r="G49" s="9">
         <v>0</v>
       </c>
-      <c r="H49" s="27">
+      <c r="H49" s="26">
         <f t="shared" si="0"/>
         <v>1029792035</v>
       </c>
@@ -5027,7 +5026,7 @@
       <c r="G50" s="9">
         <v>4.8878244293464976E-5</v>
       </c>
-      <c r="H50" s="27">
+      <c r="H50" s="26">
         <f t="shared" si="0"/>
         <v>628842026</v>
       </c>
@@ -5070,7 +5069,7 @@
       <c r="G51" s="9">
         <v>0.14049510437834842</v>
       </c>
-      <c r="H51" s="27">
+      <c r="H51" s="26">
         <f t="shared" si="0"/>
         <v>762572206</v>
       </c>
@@ -5113,7 +5112,7 @@
       <c r="G52" s="9">
         <v>0</v>
       </c>
-      <c r="H52" s="27">
+      <c r="H52" s="26">
         <f t="shared" si="0"/>
         <v>241217875</v>
       </c>
@@ -5156,7 +5155,7 @@
       <c r="G53" s="9">
         <v>8.9671956095259381E-2</v>
       </c>
-      <c r="H53" s="27">
+      <c r="H53" s="26">
         <f t="shared" si="0"/>
         <v>2424103332</v>
       </c>
@@ -5199,7 +5198,7 @@
       <c r="G54" s="9">
         <v>0</v>
       </c>
-      <c r="H54" s="27">
+      <c r="H54" s="26">
         <f t="shared" si="0"/>
         <v>1266042839</v>
       </c>
@@ -5242,7 +5241,7 @@
       <c r="G55" s="9">
         <v>0</v>
       </c>
-      <c r="H55" s="27">
+      <c r="H55" s="26">
         <f t="shared" si="0"/>
         <v>458645875</v>
       </c>
@@ -5285,7 +5284,7 @@
       <c r="G56" s="9">
         <v>0</v>
       </c>
-      <c r="H56" s="27">
+      <c r="H56" s="26">
         <f t="shared" si="0"/>
         <v>1940385286</v>
       </c>
@@ -5328,7 +5327,7 @@
       <c r="G57" s="9">
         <v>0.14597445405850845</v>
       </c>
-      <c r="H57" s="27">
+      <c r="H57" s="26">
         <f t="shared" si="0"/>
         <v>3581217780</v>
       </c>
@@ -5371,7 +5370,7 @@
       <c r="G58" s="9">
         <v>0</v>
       </c>
-      <c r="H58" s="27">
+      <c r="H58" s="26">
         <f t="shared" si="0"/>
         <v>68355867</v>
       </c>
@@ -5414,7 +5413,7 @@
       <c r="G59" s="9">
         <v>1</v>
       </c>
-      <c r="H59" s="27">
+      <c r="H59" s="26">
         <f t="shared" si="0"/>
         <v>55950828</v>
       </c>
@@ -5457,7 +5456,7 @@
       <c r="G60" s="9">
         <v>1</v>
       </c>
-      <c r="H60" s="27">
+      <c r="H60" s="26">
         <f t="shared" si="0"/>
         <v>332574215</v>
       </c>
@@ -5500,7 +5499,7 @@
       <c r="G61" s="9">
         <v>0</v>
       </c>
-      <c r="H61" s="27">
+      <c r="H61" s="26">
         <f t="shared" si="0"/>
         <v>3895740167</v>
       </c>
@@ -5543,7 +5542,7 @@
       <c r="G62" s="9">
         <v>6.9796954314720813E-3</v>
       </c>
-      <c r="H62" s="27">
+      <c r="H62" s="26">
         <f t="shared" si="0"/>
         <v>263317262</v>
       </c>
@@ -5586,7 +5585,7 @@
       <c r="G63" s="9">
         <v>0</v>
       </c>
-      <c r="H63" s="27">
+      <c r="H63" s="26">
         <f t="shared" si="0"/>
         <v>27005746</v>
       </c>
@@ -5629,7 +5628,7 @@
       <c r="G64" s="9">
         <v>0</v>
       </c>
-      <c r="H64" s="27">
+      <c r="H64" s="26">
         <f t="shared" si="0"/>
         <v>297648272</v>
       </c>
@@ -5672,7 +5671,7 @@
       <c r="G65" s="9">
         <v>0.5655287159072101</v>
       </c>
-      <c r="H65" s="27">
+      <c r="H65" s="26">
         <f t="shared" si="0"/>
         <v>4291695856</v>
       </c>
@@ -5715,7 +5714,7 @@
       <c r="G66" s="9">
         <v>2.1028891868828479E-2</v>
       </c>
-      <c r="H66" s="27">
+      <c r="H66" s="26">
         <f t="shared" ref="H66:H129" si="5">E66+F66</f>
         <v>3439722892</v>
       </c>
@@ -5758,7 +5757,7 @@
       <c r="G67" s="9">
         <v>0</v>
       </c>
-      <c r="H67" s="27">
+      <c r="H67" s="26">
         <f t="shared" si="5"/>
         <v>4012415187</v>
       </c>
@@ -5801,7 +5800,7 @@
       <c r="G68" s="9">
         <v>0.40736511561518696</v>
       </c>
-      <c r="H68" s="27">
+      <c r="H68" s="26">
         <f t="shared" si="5"/>
         <v>675404498</v>
       </c>
@@ -5844,7 +5843,7 @@
       <c r="G69" s="9">
         <v>0</v>
       </c>
-      <c r="H69" s="27">
+      <c r="H69" s="26">
         <f t="shared" si="5"/>
         <v>80878723</v>
       </c>
@@ -5887,7 +5886,7 @@
       <c r="G70" s="9">
         <v>7.9656894123671745E-2</v>
       </c>
-      <c r="H70" s="27">
+      <c r="H70" s="26">
         <f t="shared" si="5"/>
         <v>4485097322</v>
       </c>
@@ -5930,7 +5929,7 @@
       <c r="G71" s="9">
         <v>0.25718297146868574</v>
       </c>
-      <c r="H71" s="27">
+      <c r="H71" s="26">
         <f t="shared" si="5"/>
         <v>995976794</v>
       </c>
@@ -5973,7 +5972,7 @@
       <c r="G72" s="9">
         <v>0</v>
       </c>
-      <c r="H72" s="27">
+      <c r="H72" s="26">
         <f t="shared" si="5"/>
         <v>305342313</v>
       </c>
@@ -6016,7 +6015,7 @@
       <c r="G73" s="9">
         <v>1</v>
       </c>
-      <c r="H73" s="27">
+      <c r="H73" s="26">
         <f t="shared" si="5"/>
         <v>20239203</v>
       </c>
@@ -6059,7 +6058,7 @@
       <c r="G74" s="9">
         <v>0</v>
       </c>
-      <c r="H74" s="27">
+      <c r="H74" s="26">
         <f t="shared" si="5"/>
         <v>707707736</v>
       </c>
@@ -6102,7 +6101,7 @@
       <c r="G75" s="9">
         <v>0</v>
       </c>
-      <c r="H75" s="27">
+      <c r="H75" s="26">
         <f t="shared" si="5"/>
         <v>111632567</v>
       </c>
@@ -6145,7 +6144,7 @@
       <c r="G76" s="9">
         <v>0</v>
       </c>
-      <c r="H76" s="27">
+      <c r="H76" s="26">
         <f t="shared" si="5"/>
         <v>627461030</v>
       </c>
@@ -6188,7 +6187,7 @@
       <c r="G77" s="9">
         <v>0</v>
       </c>
-      <c r="H77" s="27">
+      <c r="H77" s="26">
         <f t="shared" si="5"/>
         <v>206382859</v>
       </c>
@@ -6231,7 +6230,7 @@
       <c r="G78" s="9">
         <v>0</v>
       </c>
-      <c r="H78" s="27">
+      <c r="H78" s="26">
         <f t="shared" si="5"/>
         <v>1516097702</v>
       </c>
@@ -6274,7 +6273,7 @@
       <c r="G79" s="9">
         <v>7.0179238641901773E-2</v>
       </c>
-      <c r="H79" s="27">
+      <c r="H79" s="26">
         <f t="shared" si="5"/>
         <v>1047876342</v>
       </c>
@@ -6317,7 +6316,7 @@
       <c r="G80" s="9">
         <v>0</v>
       </c>
-      <c r="H80" s="27">
+      <c r="H80" s="26">
         <f t="shared" si="5"/>
         <v>1595740380</v>
       </c>
@@ -6360,7 +6359,7 @@
       <c r="G81" s="9">
         <v>0</v>
       </c>
-      <c r="H81" s="27">
+      <c r="H81" s="26">
         <f t="shared" si="5"/>
         <v>257016401</v>
       </c>
@@ -6403,7 +6402,7 @@
       <c r="G82" s="9">
         <v>8.7741801289606874E-2</v>
       </c>
-      <c r="H82" s="27">
+      <c r="H82" s="26">
         <f t="shared" si="5"/>
         <v>1870860537</v>
       </c>
@@ -6446,7 +6445,7 @@
       <c r="G83" s="9">
         <v>0</v>
       </c>
-      <c r="H83" s="27">
+      <c r="H83" s="26">
         <f t="shared" si="5"/>
         <v>1166384803</v>
       </c>
@@ -6489,7 +6488,7 @@
       <c r="G84" s="9">
         <v>0.32653122739329637</v>
       </c>
-      <c r="H84" s="27">
+      <c r="H84" s="26">
         <f t="shared" si="5"/>
         <v>1549343656</v>
       </c>
@@ -6532,7 +6531,7 @@
       <c r="G85" s="9">
         <v>7.2703007904732581E-2</v>
       </c>
-      <c r="H85" s="27">
+      <c r="H85" s="26">
         <f t="shared" si="5"/>
         <v>4605220529</v>
       </c>
@@ -6575,7 +6574,7 @@
       <c r="G86" s="9">
         <v>0.35407527129993072</v>
       </c>
-      <c r="H86" s="27">
+      <c r="H86" s="26">
         <f t="shared" si="5"/>
         <v>152391560</v>
       </c>
@@ -6618,7 +6617,7 @@
       <c r="G87" s="9">
         <v>0</v>
       </c>
-      <c r="H87" s="27">
+      <c r="H87" s="26">
         <f t="shared" si="5"/>
         <v>6585552</v>
       </c>
@@ -6661,7 +6660,7 @@
       <c r="G88" s="9">
         <v>0</v>
       </c>
-      <c r="H88" s="27">
+      <c r="H88" s="26">
         <f t="shared" si="5"/>
         <v>49717020</v>
       </c>
@@ -6704,7 +6703,7 @@
       <c r="G89" s="9">
         <v>0.1706042921686747</v>
       </c>
-      <c r="H89" s="27">
+      <c r="H89" s="26">
         <f t="shared" si="5"/>
         <v>816197302</v>
       </c>
@@ -6747,7 +6746,7 @@
       <c r="G90" s="9">
         <v>0</v>
       </c>
-      <c r="H90" s="27">
+      <c r="H90" s="26">
         <f t="shared" si="5"/>
         <v>333568014</v>
       </c>
@@ -6790,7 +6789,7 @@
       <c r="G91" s="9">
         <v>0</v>
       </c>
-      <c r="H91" s="27">
+      <c r="H91" s="26">
         <f t="shared" si="5"/>
         <v>9717680</v>
       </c>
@@ -6833,7 +6832,7 @@
       <c r="G92" s="9">
         <v>8.7930697583534162E-4</v>
       </c>
-      <c r="H92" s="27">
+      <c r="H92" s="26">
         <f t="shared" si="5"/>
         <v>2458152004</v>
       </c>
@@ -6876,7 +6875,7 @@
       <c r="G93" s="9">
         <v>0.40862944162436549</v>
       </c>
-      <c r="H93" s="27">
+      <c r="H93" s="26">
         <f t="shared" si="5"/>
         <v>111529037</v>
       </c>
@@ -6919,7 +6918,7 @@
       <c r="G94" s="9">
         <v>0</v>
       </c>
-      <c r="H94" s="27">
+      <c r="H94" s="26">
         <f t="shared" si="5"/>
         <v>296111999</v>
       </c>
@@ -6962,7 +6961,7 @@
       <c r="G95" s="9">
         <v>0.43509474246063518</v>
       </c>
-      <c r="H95" s="27">
+      <c r="H95" s="26">
         <f t="shared" si="5"/>
         <v>1431877174</v>
       </c>
@@ -7005,7 +7004,7 @@
       <c r="G96" s="9">
         <v>0.81856584644629848</v>
       </c>
-      <c r="H96" s="27">
+      <c r="H96" s="26">
         <f t="shared" si="5"/>
         <v>255653858</v>
       </c>
@@ -7048,7 +7047,7 @@
       <c r="G97" s="9">
         <v>1</v>
       </c>
-      <c r="H97" s="27">
+      <c r="H97" s="26">
         <f t="shared" si="5"/>
         <v>320835970</v>
       </c>
@@ -7091,7 +7090,7 @@
       <c r="G98" s="9">
         <v>0</v>
       </c>
-      <c r="H98" s="27">
+      <c r="H98" s="26">
         <f t="shared" si="5"/>
         <v>510861531</v>
       </c>
@@ -7134,7 +7133,7 @@
       <c r="G99" s="9">
         <v>0</v>
       </c>
-      <c r="H99" s="27">
+      <c r="H99" s="26">
         <f t="shared" si="5"/>
         <v>503056212</v>
       </c>
@@ -7177,7 +7176,7 @@
       <c r="G100" s="9">
         <v>0.61717232102824693</v>
       </c>
-      <c r="H100" s="27">
+      <c r="H100" s="26">
         <f t="shared" si="5"/>
         <v>203059171</v>
       </c>
@@ -7220,7 +7219,7 @@
       <c r="G101" s="9">
         <v>0</v>
       </c>
-      <c r="H101" s="27">
+      <c r="H101" s="26">
         <f t="shared" si="5"/>
         <v>33858138</v>
       </c>
@@ -7263,7 +7262,7 @@
       <c r="G102" s="9">
         <v>0.34036539124439846</v>
       </c>
-      <c r="H102" s="27">
+      <c r="H102" s="26">
         <f t="shared" si="5"/>
         <v>472644046</v>
       </c>
@@ -7306,7 +7305,7 @@
       <c r="G103" s="9">
         <v>1.193001060445387E-2</v>
       </c>
-      <c r="H103" s="27">
+      <c r="H103" s="26">
         <f t="shared" si="5"/>
         <v>3311352181</v>
       </c>
@@ -7349,7 +7348,7 @@
       <c r="G104" s="9">
         <v>0.98561292865589278</v>
       </c>
-      <c r="H104" s="27">
+      <c r="H104" s="26">
         <f t="shared" si="5"/>
         <v>211526448</v>
       </c>
@@ -7392,7 +7391,7 @@
       <c r="G105" s="9">
         <v>4.807692307692308E-4</v>
       </c>
-      <c r="H105" s="27">
+      <c r="H105" s="26">
         <f t="shared" si="5"/>
         <v>534541739</v>
       </c>
@@ -7435,7 +7434,7 @@
       <c r="G106" s="9">
         <v>0</v>
       </c>
-      <c r="H106" s="27">
+      <c r="H106" s="26">
         <f t="shared" si="5"/>
         <v>2230785185</v>
       </c>
@@ -7478,7 +7477,7 @@
       <c r="G107" s="9">
         <v>0</v>
       </c>
-      <c r="H107" s="27">
+      <c r="H107" s="26">
         <f t="shared" si="5"/>
         <v>813448153</v>
       </c>
@@ -7521,7 +7520,7 @@
       <c r="G108" s="9">
         <v>9.9961926518180089E-2</v>
       </c>
-      <c r="H108" s="27">
+      <c r="H108" s="26">
         <f t="shared" si="5"/>
         <v>2349659945</v>
       </c>
@@ -7564,7 +7563,7 @@
       <c r="G109" s="9">
         <v>0</v>
       </c>
-      <c r="H109" s="27">
+      <c r="H109" s="26">
         <f t="shared" si="5"/>
         <v>11900305</v>
       </c>
@@ -7607,7 +7606,7 @@
       <c r="G110" s="9">
         <v>0</v>
       </c>
-      <c r="H110" s="27">
+      <c r="H110" s="26">
         <f t="shared" si="5"/>
         <v>1332563908</v>
       </c>
@@ -7650,7 +7649,7 @@
       <c r="G111" s="9">
         <v>1</v>
       </c>
-      <c r="H111" s="27">
+      <c r="H111" s="26">
         <f t="shared" si="5"/>
         <v>66791715</v>
       </c>
@@ -7693,7 +7692,7 @@
       <c r="G112" s="9">
         <v>0.34896984020962851</v>
       </c>
-      <c r="H112" s="27">
+      <c r="H112" s="26">
         <f t="shared" si="5"/>
         <v>864314851</v>
       </c>
@@ -7736,7 +7735,7 @@
       <c r="G113" s="9">
         <v>0</v>
       </c>
-      <c r="H113" s="27">
+      <c r="H113" s="26">
         <f t="shared" si="5"/>
         <v>1283725549</v>
       </c>
@@ -7779,7 +7778,7 @@
       <c r="G114" s="9">
         <v>0</v>
       </c>
-      <c r="H114" s="27">
+      <c r="H114" s="26">
         <f t="shared" si="5"/>
         <v>25717689</v>
       </c>
@@ -7822,7 +7821,7 @@
       <c r="G115" s="9">
         <v>0</v>
       </c>
-      <c r="H115" s="27">
+      <c r="H115" s="26">
         <f t="shared" si="5"/>
         <v>168017453</v>
       </c>
@@ -7865,7 +7864,7 @@
       <c r="G116" s="9">
         <v>0</v>
       </c>
-      <c r="H116" s="27">
+      <c r="H116" s="26">
         <f t="shared" si="5"/>
         <v>499870799</v>
       </c>
@@ -7908,7 +7907,7 @@
       <c r="G117" s="9">
         <v>0</v>
       </c>
-      <c r="H117" s="27">
+      <c r="H117" s="26">
         <f t="shared" si="5"/>
         <v>256010205</v>
       </c>
@@ -7951,7 +7950,7 @@
       <c r="G118" s="9">
         <v>0</v>
       </c>
-      <c r="H118" s="27">
+      <c r="H118" s="26">
         <f t="shared" si="5"/>
         <v>983965749</v>
       </c>
@@ -7994,7 +7993,7 @@
       <c r="G119" s="9">
         <v>0</v>
       </c>
-      <c r="H119" s="27">
+      <c r="H119" s="26">
         <f t="shared" si="5"/>
         <v>359259517</v>
       </c>
@@ -8037,7 +8036,7 @@
       <c r="G120" s="9">
         <v>0.38476476769396523</v>
       </c>
-      <c r="H120" s="27">
+      <c r="H120" s="26">
         <f t="shared" si="5"/>
         <v>5699632851</v>
       </c>
@@ -8080,7 +8079,7 @@
       <c r="G121" s="9">
         <v>0.54738095238095241</v>
       </c>
-      <c r="H121" s="27">
+      <c r="H121" s="26">
         <f t="shared" si="5"/>
         <v>192928846</v>
       </c>
@@ -8123,7 +8122,7 @@
       <c r="G122" s="9">
         <v>0</v>
       </c>
-      <c r="H122" s="27">
+      <c r="H122" s="26">
         <f t="shared" si="5"/>
         <v>12985915</v>
       </c>
@@ -8166,7 +8165,7 @@
       <c r="G123" s="9">
         <v>0</v>
       </c>
-      <c r="H123" s="27">
+      <c r="H123" s="26">
         <f t="shared" si="5"/>
         <v>329068901</v>
       </c>
@@ -8209,7 +8208,7 @@
       <c r="G124" s="9">
         <v>0</v>
       </c>
-      <c r="H124" s="27">
+      <c r="H124" s="26">
         <f t="shared" si="5"/>
         <v>501760711</v>
       </c>
@@ -8252,7 +8251,7 @@
       <c r="G125" s="9">
         <v>0</v>
       </c>
-      <c r="H125" s="27">
+      <c r="H125" s="26">
         <f t="shared" si="5"/>
         <v>873453598</v>
       </c>
@@ -8295,7 +8294,7 @@
       <c r="G126" s="9">
         <v>0.33365491651205936</v>
       </c>
-      <c r="H126" s="27">
+      <c r="H126" s="26">
         <f t="shared" si="5"/>
         <v>442340263</v>
       </c>
@@ -8338,7 +8337,7 @@
       <c r="G127" s="9">
         <v>0</v>
       </c>
-      <c r="H127" s="27">
+      <c r="H127" s="26">
         <f t="shared" si="5"/>
         <v>381052801</v>
       </c>
@@ -8381,7 +8380,7 @@
       <c r="G128" s="9">
         <v>0</v>
       </c>
-      <c r="H128" s="27">
+      <c r="H128" s="26">
         <f t="shared" si="5"/>
         <v>911862269</v>
       </c>
@@ -8424,7 +8423,7 @@
       <c r="G129" s="9">
         <v>0</v>
       </c>
-      <c r="H129" s="27">
+      <c r="H129" s="26">
         <f t="shared" si="5"/>
         <v>2689164681</v>
       </c>
@@ -8467,7 +8466,7 @@
       <c r="G130" s="9">
         <v>0</v>
       </c>
-      <c r="H130" s="27">
+      <c r="H130" s="26">
         <f t="shared" ref="H130:H193" si="10">E130+F130</f>
         <v>1031903455</v>
       </c>
@@ -8510,7 +8509,7 @@
       <c r="G131" s="9">
         <v>0</v>
       </c>
-      <c r="H131" s="27">
+      <c r="H131" s="26">
         <f t="shared" si="10"/>
         <v>295653081</v>
       </c>
@@ -8553,7 +8552,7 @@
       <c r="G132" s="9">
         <v>0</v>
       </c>
-      <c r="H132" s="27">
+      <c r="H132" s="26">
         <f t="shared" si="10"/>
         <v>1620451049</v>
       </c>
@@ -8596,7 +8595,7 @@
       <c r="G133" s="9">
         <v>0</v>
       </c>
-      <c r="H133" s="27">
+      <c r="H133" s="26">
         <f t="shared" si="10"/>
         <v>239173126</v>
       </c>
@@ -8639,7 +8638,7 @@
       <c r="G134" s="9">
         <v>0</v>
       </c>
-      <c r="H134" s="27">
+      <c r="H134" s="26">
         <f t="shared" si="10"/>
         <v>189067157</v>
       </c>
@@ -8682,7 +8681,7 @@
       <c r="G135" s="9">
         <v>0.5263103590590178</v>
       </c>
-      <c r="H135" s="27">
+      <c r="H135" s="26">
         <f t="shared" si="10"/>
         <v>797560787</v>
       </c>
@@ -8725,7 +8724,7 @@
       <c r="G136" s="9">
         <v>0</v>
       </c>
-      <c r="H136" s="27">
+      <c r="H136" s="26">
         <f t="shared" si="10"/>
         <v>903725961</v>
       </c>
@@ -8768,7 +8767,7 @@
       <c r="G137" s="9">
         <v>0</v>
       </c>
-      <c r="H137" s="27">
+      <c r="H137" s="26">
         <f t="shared" si="10"/>
         <v>2064532586</v>
       </c>
@@ -8811,7 +8810,7 @@
       <c r="G138" s="9">
         <v>0</v>
       </c>
-      <c r="H138" s="27">
+      <c r="H138" s="26">
         <f t="shared" si="10"/>
         <v>42521353</v>
       </c>
@@ -8854,7 +8853,7 @@
       <c r="G139" s="9">
         <v>0</v>
       </c>
-      <c r="H139" s="27">
+      <c r="H139" s="26">
         <f t="shared" si="10"/>
         <v>855834784</v>
       </c>
@@ -8897,7 +8896,7 @@
       <c r="G140" s="9">
         <v>0</v>
       </c>
-      <c r="H140" s="27">
+      <c r="H140" s="26">
         <f t="shared" si="10"/>
         <v>1148911414</v>
       </c>
@@ -8940,7 +8939,7 @@
       <c r="G141" s="9">
         <v>0</v>
       </c>
-      <c r="H141" s="27">
+      <c r="H141" s="26">
         <f t="shared" si="10"/>
         <v>441344816</v>
       </c>
@@ -8983,7 +8982,7 @@
       <c r="G142" s="9">
         <v>0</v>
       </c>
-      <c r="H142" s="27">
+      <c r="H142" s="26">
         <f t="shared" si="10"/>
         <v>6103642</v>
       </c>
@@ -9026,7 +9025,7 @@
       <c r="G143" s="9">
         <v>0</v>
       </c>
-      <c r="H143" s="27">
+      <c r="H143" s="26">
         <f t="shared" si="10"/>
         <v>1524718309</v>
       </c>
@@ -9069,7 +9068,7 @@
       <c r="G144" s="9">
         <v>9.1591936843718868E-3</v>
       </c>
-      <c r="H144" s="27">
+      <c r="H144" s="26">
         <f t="shared" si="10"/>
         <v>1087671783</v>
       </c>
@@ -9112,7 +9111,7 @@
       <c r="G145" s="9">
         <v>0.3023653206223581</v>
       </c>
-      <c r="H145" s="27">
+      <c r="H145" s="26">
         <f t="shared" si="10"/>
         <v>2840208432</v>
       </c>
@@ -9155,7 +9154,7 @@
       <c r="G146" s="9">
         <v>0</v>
       </c>
-      <c r="H146" s="27">
+      <c r="H146" s="26">
         <f t="shared" si="10"/>
         <v>687885609</v>
       </c>
@@ -9198,7 +9197,7 @@
       <c r="G147" s="9">
         <v>1</v>
       </c>
-      <c r="H147" s="27">
+      <c r="H147" s="26">
         <f t="shared" si="10"/>
         <v>178282362</v>
       </c>
@@ -9241,7 +9240,7 @@
       <c r="G148" s="9">
         <v>0.56891929370435423</v>
       </c>
-      <c r="H148" s="27">
+      <c r="H148" s="26">
         <f t="shared" si="10"/>
         <v>331907225</v>
       </c>
@@ -9284,7 +9283,7 @@
       <c r="G149" s="9">
         <v>0</v>
       </c>
-      <c r="H149" s="27">
+      <c r="H149" s="26">
         <f t="shared" si="10"/>
         <v>263945202</v>
       </c>
@@ -9327,7 +9326,7 @@
       <c r="G150" s="9">
         <v>0</v>
       </c>
-      <c r="H150" s="27">
+      <c r="H150" s="26">
         <f t="shared" si="10"/>
         <v>41327955</v>
       </c>
@@ -9370,7 +9369,7 @@
       <c r="G151" s="9">
         <v>0</v>
       </c>
-      <c r="H151" s="27">
+      <c r="H151" s="26">
         <f t="shared" si="10"/>
         <v>205218747</v>
       </c>
@@ -9413,7 +9412,7 @@
       <c r="G152" s="9">
         <v>1</v>
       </c>
-      <c r="H152" s="27">
+      <c r="H152" s="26">
         <f t="shared" si="10"/>
         <v>210458375</v>
       </c>
@@ -9456,7 +9455,7 @@
       <c r="G153" s="9">
         <v>0.17081738583337702</v>
       </c>
-      <c r="H153" s="27">
+      <c r="H153" s="26">
         <f t="shared" si="10"/>
         <v>986052636</v>
       </c>
@@ -9499,7 +9498,7 @@
       <c r="G154" s="9">
         <v>1</v>
       </c>
-      <c r="H154" s="27">
+      <c r="H154" s="26">
         <f t="shared" si="10"/>
         <v>292864452</v>
       </c>
@@ -9542,7 +9541,7 @@
       <c r="G155" s="9">
         <v>0</v>
       </c>
-      <c r="H155" s="27">
+      <c r="H155" s="26">
         <f t="shared" si="10"/>
         <v>205225015</v>
       </c>
@@ -9585,7 +9584,7 @@
       <c r="G156" s="9">
         <v>0</v>
       </c>
-      <c r="H156" s="27">
+      <c r="H156" s="26">
         <f t="shared" si="10"/>
         <v>17216828</v>
       </c>
@@ -9628,7 +9627,7 @@
       <c r="G157" s="9">
         <v>0</v>
       </c>
-      <c r="H157" s="27">
+      <c r="H157" s="26">
         <f t="shared" si="10"/>
         <v>1404191536</v>
       </c>
@@ -9671,7 +9670,7 @@
       <c r="G158" s="9">
         <v>0.80085497660913052</v>
       </c>
-      <c r="H158" s="27">
+      <c r="H158" s="26">
         <f t="shared" si="10"/>
         <v>1395731228</v>
       </c>
@@ -9714,7 +9713,7 @@
       <c r="G159" s="9">
         <v>0</v>
       </c>
-      <c r="H159" s="27">
+      <c r="H159" s="26">
         <f t="shared" si="10"/>
         <v>102703880</v>
       </c>
@@ -9757,7 +9756,7 @@
       <c r="G160" s="9">
         <v>0</v>
       </c>
-      <c r="H160" s="27">
+      <c r="H160" s="26">
         <f t="shared" si="10"/>
         <v>441899862</v>
       </c>
@@ -9800,7 +9799,7 @@
       <c r="G161" s="9">
         <v>0.38066317626527052</v>
       </c>
-      <c r="H161" s="27">
+      <c r="H161" s="26">
         <f t="shared" si="10"/>
         <v>366699984</v>
       </c>
@@ -9843,7 +9842,7 @@
       <c r="G162" s="9">
         <v>0</v>
       </c>
-      <c r="H162" s="27">
+      <c r="H162" s="26">
         <f t="shared" si="10"/>
         <v>11335248</v>
       </c>
@@ -9886,7 +9885,7 @@
       <c r="G163" s="9">
         <v>0</v>
       </c>
-      <c r="H163" s="27">
+      <c r="H163" s="26">
         <f t="shared" si="10"/>
         <v>12548016</v>
       </c>
@@ -9929,7 +9928,7 @@
       <c r="G164" s="9">
         <v>0</v>
       </c>
-      <c r="H164" s="27">
+      <c r="H164" s="26">
         <f t="shared" si="10"/>
         <v>658461699</v>
       </c>
@@ -9972,7 +9971,7 @@
       <c r="G165" s="9">
         <v>0</v>
       </c>
-      <c r="H165" s="27">
+      <c r="H165" s="26">
         <f t="shared" si="10"/>
         <v>1467566593</v>
       </c>
@@ -10015,7 +10014,7 @@
       <c r="G166" s="9">
         <v>0</v>
       </c>
-      <c r="H166" s="27">
+      <c r="H166" s="26">
         <f t="shared" si="10"/>
         <v>416634050</v>
       </c>
@@ -10058,7 +10057,7 @@
       <c r="G167" s="9">
         <v>7.4375678610206303E-2</v>
       </c>
-      <c r="H167" s="27">
+      <c r="H167" s="26">
         <f t="shared" si="10"/>
         <v>943563613</v>
       </c>
@@ -10101,7 +10100,7 @@
       <c r="G168" s="9">
         <v>0.29612206981064948</v>
       </c>
-      <c r="H168" s="27">
+      <c r="H168" s="26">
         <f t="shared" si="10"/>
         <v>1417963490</v>
       </c>
@@ -10144,7 +10143,7 @@
       <c r="G169" s="9">
         <v>0.32104411454302401</v>
       </c>
-      <c r="H169" s="27">
+      <c r="H169" s="26">
         <f t="shared" si="10"/>
         <v>4309265706</v>
       </c>
@@ -10187,7 +10186,7 @@
       <c r="G170" s="9">
         <v>0.17908745247148289</v>
       </c>
-      <c r="H170" s="27">
+      <c r="H170" s="26">
         <f t="shared" si="10"/>
         <v>1417629770</v>
       </c>
@@ -10230,7 +10229,7 @@
       <c r="G171" s="9">
         <v>0.16067272970442692</v>
       </c>
-      <c r="H171" s="27">
+      <c r="H171" s="26">
         <f t="shared" si="10"/>
         <v>11001349904</v>
       </c>
@@ -10273,7 +10272,7 @@
       <c r="G172" s="9">
         <v>7.4924671125156175E-2</v>
       </c>
-      <c r="H172" s="27">
+      <c r="H172" s="26">
         <f t="shared" si="10"/>
         <v>1511035113</v>
       </c>
@@ -10316,7 +10315,7 @@
       <c r="G173" s="9">
         <v>0</v>
       </c>
-      <c r="H173" s="27">
+      <c r="H173" s="26">
         <f t="shared" si="10"/>
         <v>32074855</v>
       </c>
@@ -10359,7 +10358,7 @@
       <c r="G174" s="9">
         <v>0.32767210144927539</v>
       </c>
-      <c r="H174" s="27">
+      <c r="H174" s="26">
         <f t="shared" si="10"/>
         <v>2956628676</v>
       </c>
@@ -10402,7 +10401,7 @@
       <c r="G175" s="9">
         <v>0</v>
       </c>
-      <c r="H175" s="27">
+      <c r="H175" s="26">
         <f t="shared" si="10"/>
         <v>949305740</v>
       </c>
@@ -10445,7 +10444,7 @@
       <c r="G176" s="9">
         <v>1.965938338535677E-2</v>
       </c>
-      <c r="H176" s="27">
+      <c r="H176" s="26">
         <f t="shared" si="10"/>
         <v>1048645605</v>
       </c>
@@ -10488,7 +10487,7 @@
       <c r="G177" s="9">
         <v>0</v>
       </c>
-      <c r="H177" s="27">
+      <c r="H177" s="26">
         <f t="shared" si="10"/>
         <v>262750137</v>
       </c>
@@ -10531,7 +10530,7 @@
       <c r="G178" s="9">
         <v>0.58269124483890888</v>
       </c>
-      <c r="H178" s="27">
+      <c r="H178" s="26">
         <f t="shared" si="10"/>
         <v>433408980</v>
       </c>
@@ -10574,7 +10573,7 @@
       <c r="G179" s="9">
         <v>0</v>
       </c>
-      <c r="H179" s="27">
+      <c r="H179" s="26">
         <f t="shared" si="10"/>
         <v>810792565</v>
       </c>
@@ -10617,7 +10616,7 @@
       <c r="G180" s="9">
         <v>1.371302027142127E-2</v>
       </c>
-      <c r="H180" s="27">
+      <c r="H180" s="26">
         <f t="shared" si="10"/>
         <v>3771496836</v>
       </c>
@@ -10660,7 +10659,7 @@
       <c r="G181" s="9">
         <v>0</v>
       </c>
-      <c r="H181" s="27">
+      <c r="H181" s="26">
         <f t="shared" si="10"/>
         <v>884289868</v>
       </c>
@@ -10703,7 +10702,7 @@
       <c r="G182" s="9">
         <v>0.20973520249221184</v>
       </c>
-      <c r="H182" s="27">
+      <c r="H182" s="26">
         <f t="shared" si="10"/>
         <v>755309217</v>
       </c>
@@ -10746,7 +10745,7 @@
       <c r="G183" s="9">
         <v>0</v>
       </c>
-      <c r="H183" s="27">
+      <c r="H183" s="26">
         <f t="shared" si="10"/>
         <v>2859155028</v>
       </c>
@@ -10789,7 +10788,7 @@
       <c r="G184" s="9">
         <v>7.4568745905815567E-2</v>
       </c>
-      <c r="H184" s="27">
+      <c r="H184" s="26">
         <f t="shared" si="10"/>
         <v>658539294</v>
       </c>
@@ -10832,7 +10831,7 @@
       <c r="G185" s="9">
         <v>0.36803056783523524</v>
       </c>
-      <c r="H185" s="27">
+      <c r="H185" s="26">
         <f t="shared" si="10"/>
         <v>2343399604</v>
       </c>
@@ -10875,7 +10874,7 @@
       <c r="G186" s="9">
         <v>0</v>
       </c>
-      <c r="H186" s="27">
+      <c r="H186" s="26">
         <f t="shared" si="10"/>
         <v>2109573717</v>
       </c>
@@ -10918,7 +10917,7 @@
       <c r="G187" s="9">
         <v>0.5136314067611778</v>
       </c>
-      <c r="H187" s="27">
+      <c r="H187" s="26">
         <f t="shared" si="10"/>
         <v>537355757</v>
       </c>
@@ -10961,7 +10960,7 @@
       <c r="G188" s="9">
         <v>0</v>
       </c>
-      <c r="H188" s="27">
+      <c r="H188" s="26">
         <f t="shared" si="10"/>
         <v>58521853</v>
       </c>
@@ -11004,7 +11003,7 @@
       <c r="G189" s="9">
         <v>0</v>
       </c>
-      <c r="H189" s="27">
+      <c r="H189" s="26">
         <f t="shared" si="10"/>
         <v>8446899</v>
       </c>
@@ -11047,7 +11046,7 @@
       <c r="G190" s="9">
         <v>0</v>
       </c>
-      <c r="H190" s="27">
+      <c r="H190" s="26">
         <f t="shared" si="10"/>
         <v>253440039</v>
       </c>
@@ -11090,7 +11089,7 @@
       <c r="G191" s="9">
         <v>0</v>
       </c>
-      <c r="H191" s="27">
+      <c r="H191" s="26">
         <f t="shared" si="10"/>
         <v>306555546</v>
       </c>
@@ -11133,7 +11132,7 @@
       <c r="G192" s="9">
         <v>0</v>
       </c>
-      <c r="H192" s="27">
+      <c r="H192" s="26">
         <f t="shared" si="10"/>
         <v>4368853853</v>
       </c>
@@ -11176,7 +11175,7 @@
       <c r="G193" s="9">
         <v>0.10371548359115224</v>
       </c>
-      <c r="H193" s="27">
+      <c r="H193" s="26">
         <f t="shared" si="10"/>
         <v>1629036457</v>
       </c>
@@ -11219,7 +11218,7 @@
       <c r="G194" s="9">
         <v>0.18455852035106321</v>
       </c>
-      <c r="H194" s="27">
+      <c r="H194" s="26">
         <f t="shared" ref="H194:H257" si="15">E194+F194</f>
         <v>2857087147</v>
       </c>
@@ -11262,7 +11261,7 @@
       <c r="G195" s="9">
         <v>0</v>
       </c>
-      <c r="H195" s="27">
+      <c r="H195" s="26">
         <f t="shared" si="15"/>
         <v>565260098</v>
       </c>
@@ -11305,7 +11304,7 @@
       <c r="G196" s="9">
         <v>0.39136535348084189</v>
       </c>
-      <c r="H196" s="27">
+      <c r="H196" s="26">
         <f t="shared" si="15"/>
         <v>436851810</v>
       </c>
@@ -11348,7 +11347,7 @@
       <c r="G197" s="9">
         <v>0</v>
       </c>
-      <c r="H197" s="27">
+      <c r="H197" s="26">
         <f t="shared" si="15"/>
         <v>310360399</v>
       </c>
@@ -11391,7 +11390,7 @@
       <c r="G198" s="9">
         <v>0.79746353836398221</v>
       </c>
-      <c r="H198" s="27">
+      <c r="H198" s="26">
         <f t="shared" si="15"/>
         <v>86999825</v>
       </c>
@@ -11434,7 +11433,7 @@
       <c r="G199" s="9">
         <v>0.89717342186563376</v>
       </c>
-      <c r="H199" s="27">
+      <c r="H199" s="26">
         <f t="shared" si="15"/>
         <v>163093261</v>
       </c>
@@ -11477,7 +11476,7 @@
       <c r="G200" s="9">
         <v>1.7525721202340125E-2</v>
       </c>
-      <c r="H200" s="27">
+      <c r="H200" s="26">
         <f t="shared" si="15"/>
         <v>2212089003</v>
       </c>
@@ -11520,7 +11519,7 @@
       <c r="G201" s="9">
         <v>0</v>
       </c>
-      <c r="H201" s="27">
+      <c r="H201" s="26">
         <f t="shared" si="15"/>
         <v>194555133</v>
       </c>
@@ -11563,7 +11562,7 @@
       <c r="G202" s="9">
         <v>1</v>
       </c>
-      <c r="H202" s="27">
+      <c r="H202" s="26">
         <f t="shared" si="15"/>
         <v>19985861</v>
       </c>
@@ -11606,7 +11605,7 @@
       <c r="G203" s="9">
         <v>0</v>
       </c>
-      <c r="H203" s="27">
+      <c r="H203" s="26">
         <f t="shared" si="15"/>
         <v>277195200</v>
       </c>
@@ -11649,7 +11648,7 @@
       <c r="G204" s="9">
         <v>0</v>
       </c>
-      <c r="H204" s="27">
+      <c r="H204" s="26">
         <f t="shared" si="15"/>
         <v>2047820152</v>
       </c>
@@ -11692,7 +11691,7 @@
       <c r="G205" s="9">
         <v>0</v>
       </c>
-      <c r="H205" s="27">
+      <c r="H205" s="26">
         <f t="shared" si="15"/>
         <v>405832154</v>
       </c>
@@ -11735,7 +11734,7 @@
       <c r="G206" s="9">
         <v>0</v>
       </c>
-      <c r="H206" s="27">
+      <c r="H206" s="26">
         <f t="shared" si="15"/>
         <v>6291402</v>
       </c>
@@ -11778,7 +11777,7 @@
       <c r="G207" s="9">
         <v>0</v>
       </c>
-      <c r="H207" s="27">
+      <c r="H207" s="26">
         <f t="shared" si="15"/>
         <v>54740336</v>
       </c>
@@ -11821,7 +11820,7 @@
       <c r="G208" s="9">
         <v>1</v>
       </c>
-      <c r="H208" s="27">
+      <c r="H208" s="26">
         <f t="shared" si="15"/>
         <v>102285801</v>
       </c>
@@ -11864,7 +11863,7 @@
       <c r="G209" s="9">
         <v>0</v>
       </c>
-      <c r="H209" s="27">
+      <c r="H209" s="26">
         <f t="shared" si="15"/>
         <v>139272393</v>
       </c>
@@ -11907,7 +11906,7 @@
       <c r="G210" s="9">
         <v>0.28926391829617637</v>
       </c>
-      <c r="H210" s="27">
+      <c r="H210" s="26">
         <f t="shared" si="15"/>
         <v>551198083</v>
       </c>
@@ -11950,7 +11949,7 @@
       <c r="G211" s="9">
         <v>0</v>
       </c>
-      <c r="H211" s="27">
+      <c r="H211" s="26">
         <f t="shared" si="15"/>
         <v>92096820</v>
       </c>
@@ -11993,7 +11992,7 @@
       <c r="G212" s="9">
         <v>0.32790606653620352</v>
       </c>
-      <c r="H212" s="27">
+      <c r="H212" s="26">
         <f t="shared" si="15"/>
         <v>248719982</v>
       </c>
@@ -12036,7 +12035,7 @@
       <c r="G213" s="9">
         <v>0</v>
       </c>
-      <c r="H213" s="27">
+      <c r="H213" s="26">
         <f t="shared" si="15"/>
         <v>40323770</v>
       </c>
@@ -12079,7 +12078,7 @@
       <c r="G214" s="9">
         <v>0</v>
       </c>
-      <c r="H214" s="27">
+      <c r="H214" s="26">
         <f t="shared" si="15"/>
         <v>741034570</v>
       </c>
@@ -12122,7 +12121,7 @@
       <c r="G215" s="9">
         <v>0.63164342254052019</v>
       </c>
-      <c r="H215" s="27">
+      <c r="H215" s="26">
         <f t="shared" si="15"/>
         <v>347465848</v>
       </c>
@@ -12165,7 +12164,7 @@
       <c r="G216" s="9">
         <v>1</v>
       </c>
-      <c r="H216" s="27">
+      <c r="H216" s="26">
         <f t="shared" si="15"/>
         <v>134006945</v>
       </c>
@@ -12208,7 +12207,7 @@
       <c r="G217" s="9">
         <v>0</v>
       </c>
-      <c r="H217" s="27">
+      <c r="H217" s="26">
         <f t="shared" si="15"/>
         <v>327653194</v>
       </c>
@@ -12251,7 +12250,7 @@
       <c r="G218" s="9">
         <v>0</v>
       </c>
-      <c r="H218" s="27">
+      <c r="H218" s="26">
         <f t="shared" si="15"/>
         <v>411153551</v>
       </c>
@@ -12294,7 +12293,7 @@
       <c r="G219" s="9">
         <v>1</v>
       </c>
-      <c r="H219" s="27">
+      <c r="H219" s="26">
         <f t="shared" si="15"/>
         <v>45487175</v>
       </c>
@@ -12337,7 +12336,7 @@
       <c r="G220" s="9">
         <v>0</v>
       </c>
-      <c r="H220" s="27">
+      <c r="H220" s="26">
         <f t="shared" si="15"/>
         <v>146185927</v>
       </c>
@@ -12380,7 +12379,7 @@
       <c r="G221" s="9">
         <v>5.37603305785124E-2</v>
       </c>
-      <c r="H221" s="27">
+      <c r="H221" s="26">
         <f t="shared" si="15"/>
         <v>1287287019</v>
       </c>
@@ -12423,7 +12422,7 @@
       <c r="G222" s="9">
         <v>0.3603592303639967</v>
       </c>
-      <c r="H222" s="27">
+      <c r="H222" s="26">
         <f t="shared" si="15"/>
         <v>2031127269</v>
       </c>
@@ -12466,7 +12465,7 @@
       <c r="G223" s="9">
         <v>0</v>
       </c>
-      <c r="H223" s="27">
+      <c r="H223" s="26">
         <f t="shared" si="15"/>
         <v>1130248997</v>
       </c>
@@ -12509,7 +12508,7 @@
       <c r="G224" s="9">
         <v>0.35804655870445345</v>
       </c>
-      <c r="H224" s="27">
+      <c r="H224" s="26">
         <f t="shared" si="15"/>
         <v>1309163373</v>
       </c>
@@ -12552,7 +12551,7 @@
       <c r="G225" s="9">
         <v>0.53351850862667594</v>
       </c>
-      <c r="H225" s="27">
+      <c r="H225" s="26">
         <f t="shared" si="15"/>
         <v>396054910</v>
       </c>
@@ -12595,7 +12594,7 @@
       <c r="G226" s="9">
         <v>0.63518273888154997</v>
       </c>
-      <c r="H226" s="27">
+      <c r="H226" s="26">
         <f t="shared" si="15"/>
         <v>805463127</v>
       </c>
@@ -12638,7 +12637,7 @@
       <c r="G227" s="9">
         <v>0.41952707856598015</v>
       </c>
-      <c r="H227" s="27">
+      <c r="H227" s="26">
         <f t="shared" si="15"/>
         <v>48687098</v>
       </c>
@@ -12681,7 +12680,7 @@
       <c r="G228" s="9">
         <v>0.71015625000000004</v>
       </c>
-      <c r="H228" s="27">
+      <c r="H228" s="26">
         <f t="shared" si="15"/>
         <v>109213950</v>
       </c>
@@ -12724,7 +12723,7 @@
       <c r="G229" s="9">
         <v>0</v>
       </c>
-      <c r="H229" s="27">
+      <c r="H229" s="26">
         <f t="shared" si="15"/>
         <v>285302418</v>
       </c>
@@ -12767,7 +12766,7 @@
       <c r="G230" s="9">
         <v>1</v>
       </c>
-      <c r="H230" s="27">
+      <c r="H230" s="26">
         <f t="shared" si="15"/>
         <v>109971653</v>
       </c>
@@ -12810,7 +12809,7 @@
       <c r="G231" s="9">
         <v>0.18863610380701956</v>
       </c>
-      <c r="H231" s="27">
+      <c r="H231" s="26">
         <f t="shared" si="15"/>
         <v>7146099477</v>
       </c>
@@ -12853,7 +12852,7 @@
       <c r="G232" s="9">
         <v>0</v>
       </c>
-      <c r="H232" s="27">
+      <c r="H232" s="26">
         <f t="shared" si="15"/>
         <v>660198438</v>
       </c>
@@ -12896,7 +12895,7 @@
       <c r="G233" s="9">
         <v>0</v>
       </c>
-      <c r="H233" s="27">
+      <c r="H233" s="26">
         <f t="shared" si="15"/>
         <v>1066423597</v>
       </c>
@@ -12939,7 +12938,7 @@
       <c r="G234" s="9">
         <v>9.7531847133757968E-2</v>
       </c>
-      <c r="H234" s="27">
+      <c r="H234" s="26">
         <f t="shared" si="15"/>
         <v>4281475924</v>
       </c>
@@ -12982,7 +12981,7 @@
       <c r="G235" s="9">
         <v>0</v>
       </c>
-      <c r="H235" s="27">
+      <c r="H235" s="26">
         <f t="shared" si="15"/>
         <v>116793366</v>
       </c>
@@ -13025,7 +13024,7 @@
       <c r="G236" s="9">
         <v>0</v>
       </c>
-      <c r="H236" s="27">
+      <c r="H236" s="26">
         <f t="shared" si="15"/>
         <v>589827543</v>
       </c>
@@ -13068,7 +13067,7 @@
       <c r="G237" s="9">
         <v>1</v>
       </c>
-      <c r="H237" s="27">
+      <c r="H237" s="26">
         <f t="shared" si="15"/>
         <v>154559290</v>
       </c>
@@ -13111,7 +13110,7 @@
       <c r="G238" s="9">
         <v>0</v>
       </c>
-      <c r="H238" s="27">
+      <c r="H238" s="26">
         <f t="shared" si="15"/>
         <v>1120841279</v>
       </c>
@@ -13154,7 +13153,7 @@
       <c r="G239" s="9">
         <v>0.53640810621942703</v>
       </c>
-      <c r="H239" s="27">
+      <c r="H239" s="26">
         <f t="shared" si="15"/>
         <v>615570621</v>
       </c>
@@ -13197,7 +13196,7 @@
       <c r="G240" s="9">
         <v>0</v>
       </c>
-      <c r="H240" s="27">
+      <c r="H240" s="26">
         <f t="shared" si="15"/>
         <v>263440807</v>
       </c>
@@ -13240,7 +13239,7 @@
       <c r="G241" s="9">
         <v>0</v>
       </c>
-      <c r="H241" s="27">
+      <c r="H241" s="26">
         <f t="shared" si="15"/>
         <v>2759668613</v>
       </c>
@@ -13283,7 +13282,7 @@
       <c r="G242" s="9">
         <v>0.23069699499165275</v>
       </c>
-      <c r="H242" s="27">
+      <c r="H242" s="26">
         <f t="shared" si="15"/>
         <v>156526015</v>
       </c>
@@ -13326,7 +13325,7 @@
       <c r="G243" s="9">
         <v>1</v>
       </c>
-      <c r="H243" s="27">
+      <c r="H243" s="26">
         <f t="shared" si="15"/>
         <v>154888140</v>
       </c>
@@ -13369,7 +13368,7 @@
       <c r="G244" s="9">
         <v>1</v>
       </c>
-      <c r="H244" s="27">
+      <c r="H244" s="26">
         <f t="shared" si="15"/>
         <v>84702806</v>
       </c>
@@ -13412,7 +13411,7 @@
       <c r="G245" s="9">
         <v>0.26090911387927329</v>
       </c>
-      <c r="H245" s="27">
+      <c r="H245" s="26">
         <f t="shared" si="15"/>
         <v>1315089966</v>
       </c>
@@ -13455,7 +13454,7 @@
       <c r="G246" s="9">
         <v>0</v>
       </c>
-      <c r="H246" s="27">
+      <c r="H246" s="26">
         <f t="shared" si="15"/>
         <v>431214431</v>
       </c>
@@ -13498,7 +13497,7 @@
       <c r="G247" s="9">
         <v>0.99847683899292183</v>
       </c>
-      <c r="H247" s="27">
+      <c r="H247" s="26">
         <f t="shared" si="15"/>
         <v>274147933</v>
       </c>
@@ -13541,7 +13540,7 @@
       <c r="G248" s="9">
         <v>0</v>
       </c>
-      <c r="H248" s="27">
+      <c r="H248" s="26">
         <f t="shared" si="15"/>
         <v>12473476</v>
       </c>
@@ -13584,7 +13583,7 @@
       <c r="G249" s="9">
         <v>0</v>
       </c>
-      <c r="H249" s="27">
+      <c r="H249" s="26">
         <f t="shared" si="15"/>
         <v>74986292</v>
       </c>
@@ -13627,7 +13626,7 @@
       <c r="G250" s="9">
         <v>0</v>
       </c>
-      <c r="H250" s="27">
+      <c r="H250" s="26">
         <f t="shared" si="15"/>
         <v>74651522</v>
       </c>
@@ -13670,7 +13669,7 @@
       <c r="G251" s="9">
         <v>9.1672473245073341E-2</v>
       </c>
-      <c r="H251" s="27">
+      <c r="H251" s="26">
         <f t="shared" si="15"/>
         <v>2957663576</v>
       </c>
@@ -13713,7 +13712,7 @@
       <c r="G252" s="9">
         <v>0</v>
       </c>
-      <c r="H252" s="27">
+      <c r="H252" s="26">
         <f t="shared" si="15"/>
         <v>64469359</v>
       </c>
@@ -13756,7 +13755,7 @@
       <c r="G253" s="9">
         <v>0</v>
       </c>
-      <c r="H253" s="27">
+      <c r="H253" s="26">
         <f t="shared" si="15"/>
         <v>22871923</v>
       </c>
@@ -13799,7 +13798,7 @@
       <c r="G254" s="9">
         <v>0</v>
       </c>
-      <c r="H254" s="27">
+      <c r="H254" s="26">
         <f t="shared" si="15"/>
         <v>35423416</v>
       </c>
@@ -13842,7 +13841,7 @@
       <c r="G255" s="9">
         <v>0.4489853044086774</v>
       </c>
-      <c r="H255" s="27">
+      <c r="H255" s="26">
         <f t="shared" si="15"/>
         <v>164019622</v>
       </c>
@@ -13885,7 +13884,7 @@
       <c r="G256" s="9">
         <v>0</v>
       </c>
-      <c r="H256" s="27">
+      <c r="H256" s="26">
         <f t="shared" si="15"/>
         <v>2842772334</v>
       </c>
@@ -13928,7 +13927,7 @@
       <c r="G257" s="9">
         <v>0.23321205587746485</v>
       </c>
-      <c r="H257" s="27">
+      <c r="H257" s="26">
         <f t="shared" si="15"/>
         <v>1219669121</v>
       </c>
@@ -13971,7 +13970,7 @@
       <c r="G258" s="9">
         <v>0</v>
       </c>
-      <c r="H258" s="27">
+      <c r="H258" s="26">
         <f t="shared" ref="H258:H285" si="20">E258+F258</f>
         <v>9432267</v>
       </c>
@@ -14014,7 +14013,7 @@
       <c r="G259" s="9">
         <v>0</v>
       </c>
-      <c r="H259" s="27">
+      <c r="H259" s="26">
         <f t="shared" si="20"/>
         <v>252412479</v>
       </c>
@@ -14057,7 +14056,7 @@
       <c r="G260" s="9">
         <v>0</v>
       </c>
-      <c r="H260" s="27">
+      <c r="H260" s="26">
         <f t="shared" si="20"/>
         <v>191349398</v>
       </c>
@@ -14100,7 +14099,7 @@
       <c r="G261" s="9">
         <v>0</v>
       </c>
-      <c r="H261" s="27">
+      <c r="H261" s="26">
         <f t="shared" si="20"/>
         <v>728771445</v>
       </c>
@@ -14143,7 +14142,7 @@
       <c r="G262" s="9">
         <v>0.17963646691280885</v>
       </c>
-      <c r="H262" s="27">
+      <c r="H262" s="26">
         <f t="shared" si="20"/>
         <v>588557573</v>
       </c>
@@ -14186,7 +14185,7 @@
       <c r="G263" s="9">
         <v>0.84672137571231854</v>
       </c>
-      <c r="H263" s="27">
+      <c r="H263" s="26">
         <f t="shared" si="20"/>
         <v>2291335661</v>
       </c>
@@ -14229,7 +14228,7 @@
       <c r="G264" s="9">
         <v>0</v>
       </c>
-      <c r="H264" s="27">
+      <c r="H264" s="26">
         <f t="shared" si="20"/>
         <v>152496764</v>
       </c>
@@ -14272,7 +14271,7 @@
       <c r="G265" s="9">
         <v>0.25650035137034433</v>
       </c>
-      <c r="H265" s="27">
+      <c r="H265" s="26">
         <f t="shared" si="20"/>
         <v>1100781765</v>
       </c>
@@ -14315,7 +14314,7 @@
       <c r="G266" s="9">
         <v>0</v>
       </c>
-      <c r="H266" s="27">
+      <c r="H266" s="26">
         <f t="shared" si="20"/>
         <v>410770472</v>
       </c>
@@ -14358,7 +14357,7 @@
       <c r="G267" s="9">
         <v>0.13793511721524981</v>
       </c>
-      <c r="H267" s="27">
+      <c r="H267" s="26">
         <f t="shared" si="20"/>
         <v>658511205</v>
       </c>
@@ -14401,7 +14400,7 @@
       <c r="G268" s="9">
         <v>0</v>
       </c>
-      <c r="H268" s="27">
+      <c r="H268" s="26">
         <f t="shared" si="20"/>
         <v>853293097</v>
       </c>
@@ -14444,7 +14443,7 @@
       <c r="G269" s="9">
         <v>0</v>
       </c>
-      <c r="H269" s="27">
+      <c r="H269" s="26">
         <f t="shared" si="20"/>
         <v>1897939888</v>
       </c>
@@ -14487,7 +14486,7 @@
       <c r="G270" s="9">
         <v>0</v>
       </c>
-      <c r="H270" s="27">
+      <c r="H270" s="26">
         <f t="shared" si="20"/>
         <v>2878375603</v>
       </c>
@@ -14530,7 +14529,7 @@
       <c r="G271" s="9">
         <v>0.57822520888162099</v>
       </c>
-      <c r="H271" s="27">
+      <c r="H271" s="26">
         <f t="shared" si="20"/>
         <v>1662545938</v>
       </c>
@@ -14573,7 +14572,7 @@
       <c r="G272" s="9">
         <v>0</v>
       </c>
-      <c r="H272" s="27">
+      <c r="H272" s="26">
         <f t="shared" si="20"/>
         <v>210593587</v>
       </c>
@@ -14616,7 +14615,7 @@
       <c r="G273" s="9">
         <v>0</v>
       </c>
-      <c r="H273" s="27">
+      <c r="H273" s="26">
         <f t="shared" si="20"/>
         <v>895226920</v>
       </c>
@@ -14659,7 +14658,7 @@
       <c r="G274" s="9">
         <v>0</v>
       </c>
-      <c r="H274" s="27">
+      <c r="H274" s="26">
         <f t="shared" si="20"/>
         <v>2325326414</v>
       </c>
@@ -14702,7 +14701,7 @@
       <c r="G275" s="9">
         <v>0</v>
       </c>
-      <c r="H275" s="27">
+      <c r="H275" s="26">
         <f t="shared" si="20"/>
         <v>244931427</v>
       </c>
@@ -14745,7 +14744,7 @@
       <c r="G276" s="9">
         <v>0</v>
       </c>
-      <c r="H276" s="27">
+      <c r="H276" s="26">
         <f t="shared" si="20"/>
         <v>444601881</v>
       </c>
@@ -14788,7 +14787,7 @@
       <c r="G277" s="9">
         <v>0</v>
       </c>
-      <c r="H277" s="27">
+      <c r="H277" s="26">
         <f t="shared" si="20"/>
         <v>1624297790</v>
       </c>
@@ -14831,7 +14830,7 @@
       <c r="G278" s="9">
         <v>0.44310216256524981</v>
       </c>
-      <c r="H278" s="27">
+      <c r="H278" s="26">
         <f t="shared" si="20"/>
         <v>164915986</v>
       </c>
@@ -14874,7 +14873,7 @@
       <c r="G279" s="9">
         <v>0</v>
       </c>
-      <c r="H279" s="27">
+      <c r="H279" s="26">
         <f t="shared" si="20"/>
         <v>91617796</v>
       </c>
@@ -14917,7 +14916,7 @@
       <c r="G280" s="9">
         <v>5.6308878104481874E-2</v>
       </c>
-      <c r="H280" s="27">
+      <c r="H280" s="26">
         <f t="shared" si="20"/>
         <v>973474695</v>
       </c>
@@ -14960,7 +14959,7 @@
       <c r="G281" s="9">
         <v>0</v>
       </c>
-      <c r="H281" s="27">
+      <c r="H281" s="26">
         <f t="shared" si="20"/>
         <v>1773829829</v>
       </c>
@@ -15003,7 +15002,7 @@
       <c r="G282" s="9">
         <v>0.18306671868903629</v>
       </c>
-      <c r="H282" s="27">
+      <c r="H282" s="26">
         <f t="shared" si="20"/>
         <v>973265597</v>
       </c>
@@ -15046,7 +15045,7 @@
       <c r="G283" s="9">
         <v>0</v>
       </c>
-      <c r="H283" s="27">
+      <c r="H283" s="26">
         <f t="shared" si="20"/>
         <v>264445093</v>
       </c>
@@ -15089,7 +15088,7 @@
       <c r="G284" s="9">
         <v>0</v>
       </c>
-      <c r="H284" s="27">
+      <c r="H284" s="26">
         <f t="shared" si="20"/>
         <v>870868231</v>
       </c>
@@ -15132,7 +15131,7 @@
       <c r="G285" s="9">
         <v>0.46278645305211924</v>
       </c>
-      <c r="H285" s="27">
+      <c r="H285" s="26">
         <f t="shared" si="20"/>
         <v>513642149</v>
       </c>
@@ -15164,7 +15163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -15174,7 +15173,7 @@
     <col min="4" max="4" width="13.6640625" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" style="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="17" customWidth="1"/>
-    <col min="7" max="7" width="19" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.109375" style="8"/>
     <col min="10" max="10" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
@@ -15187,16 +15186,16 @@
       <c r="B1" s="14" t="s">
         <v>376</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>379</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>378</v>
       </c>
       <c r="G1" s="6" t="s">
@@ -15231,7 +15230,7 @@
       <c r="F2" s="17">
         <v>48396</v>
       </c>
-      <c r="G2" s="18">
+      <c r="G2" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E2/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F2)</f>
         <v>30630.861297395008</v>
       </c>
@@ -15267,7 +15266,7 @@
       <c r="F3" s="17">
         <v>14196</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E3/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F3)</f>
         <v>30500.064186940464</v>
       </c>
@@ -15303,7 +15302,7 @@
       <c r="F4" s="17">
         <v>13890</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E4/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F4)</f>
         <v>35791.134046073465</v>
       </c>
@@ -15339,7 +15338,7 @@
       <c r="F5" s="17">
         <v>41098</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E5/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F5)</f>
         <v>28812.770840513611</v>
       </c>
@@ -15375,7 +15374,7 @@
       <c r="F6" s="17">
         <v>44878</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E6/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F6)</f>
         <v>22471.516503492025</v>
       </c>
@@ -15411,7 +15410,7 @@
       <c r="F7" s="17">
         <v>96557</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E7/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F7)</f>
         <v>24391.009301096856</v>
       </c>
@@ -15447,7 +15446,7 @@
       <c r="F8" s="17">
         <v>9458</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E8/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F8)</f>
         <v>29306.018460002793</v>
       </c>
@@ -15483,7 +15482,7 @@
       <c r="F9" s="17">
         <v>36257</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E9/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F9)</f>
         <v>38298.210005806766</v>
       </c>
@@ -15519,7 +15518,7 @@
       <c r="F10" s="17">
         <v>78116</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E10/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F10)</f>
         <v>26037.689618261629</v>
       </c>
@@ -15555,7 +15554,7 @@
       <c r="F11" s="17">
         <v>20027</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E11/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F11)</f>
         <v>45230.58903267108</v>
       </c>
@@ -15591,7 +15590,7 @@
       <c r="F12" s="17">
         <v>33702</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E12/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F12)</f>
         <v>37814.920000420389</v>
       </c>
@@ -15627,7 +15626,7 @@
       <c r="F13" s="17">
         <v>45053</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E13/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F13)</f>
         <v>22202.85657816512</v>
       </c>
@@ -15663,7 +15662,7 @@
       <c r="F14" s="17">
         <v>2527</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E14/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F14)</f>
         <v>30708.30337338083</v>
       </c>
@@ -15699,7 +15698,7 @@
       <c r="F15" s="17">
         <v>13088</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E15/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F15)</f>
         <v>28918.825061841751</v>
       </c>
@@ -15735,7 +15734,7 @@
       <c r="F16" s="17">
         <v>31710</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E16/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F16)</f>
         <v>25892.048183992156</v>
       </c>
@@ -15771,7 +15770,7 @@
       <c r="F17" s="17">
         <v>55931</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E17/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F17)</f>
         <v>19953.639525161954</v>
       </c>
@@ -15807,7 +15806,7 @@
       <c r="F18" s="17">
         <v>24473</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E18/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F18)</f>
         <v>31735.261795545077</v>
       </c>
@@ -15843,7 +15842,7 @@
       <c r="F19" s="17">
         <v>20291</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E19/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F19)</f>
         <v>27723.070207587116</v>
       </c>
@@ -15879,7 +15878,7 @@
       <c r="F20" s="17">
         <v>43147</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G20" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E20/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F20)</f>
         <v>36913.600030442023</v>
       </c>
@@ -15915,7 +15914,7 @@
       <c r="F21" s="17">
         <v>19992</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E21/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F21)</f>
         <v>23701.938927013507</v>
       </c>
@@ -15951,7 +15950,7 @@
       <c r="F22" s="17">
         <v>21724</v>
       </c>
-      <c r="G22" s="18">
+      <c r="G22" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E22/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F22)</f>
         <v>21580.099824705372</v>
       </c>
@@ -15987,7 +15986,7 @@
       <c r="F23" s="17">
         <v>56296</v>
       </c>
-      <c r="G23" s="18">
+      <c r="G23" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E23/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F23)</f>
         <v>40596.586213406612</v>
       </c>
@@ -16023,7 +16022,7 @@
       <c r="F24" s="17">
         <v>11525</v>
       </c>
-      <c r="G24" s="18">
+      <c r="G24" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E24/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F24)</f>
         <v>53819.081650148248</v>
       </c>
@@ -16059,7 +16058,7 @@
       <c r="F25" s="17">
         <v>24369</v>
       </c>
-      <c r="G25" s="18">
+      <c r="G25" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E25/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F25)</f>
         <v>19990.299549639258</v>
       </c>
@@ -16095,7 +16094,7 @@
       <c r="F26" s="17">
         <v>19596</v>
       </c>
-      <c r="G26" s="18">
+      <c r="G26" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E26/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F26)</f>
         <v>59397.336350096171</v>
       </c>
@@ -16131,7 +16130,7 @@
       <c r="F27" s="17">
         <v>2567</v>
       </c>
-      <c r="G27" s="18">
+      <c r="G27" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E27/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F27)</f>
         <v>25615.440199126599</v>
       </c>
@@ -16167,7 +16166,7 @@
       <c r="F28" s="17">
         <v>39540</v>
       </c>
-      <c r="G28" s="18">
+      <c r="G28" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E28/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F28)</f>
         <v>19733.567665971757</v>
       </c>
@@ -16203,7 +16202,7 @@
       <c r="F29" s="17">
         <v>35439</v>
       </c>
-      <c r="G29" s="18">
+      <c r="G29" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E29/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F29)</f>
         <v>35586.604061517966</v>
       </c>
@@ -16239,7 +16238,7 @@
       <c r="F30" s="17">
         <v>24589</v>
       </c>
-      <c r="G30" s="18">
+      <c r="G30" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E30/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F30)</f>
         <v>26560.767292648867</v>
       </c>
@@ -16275,7 +16274,7 @@
       <c r="F31" s="17">
         <v>31471</v>
       </c>
-      <c r="G31" s="18">
+      <c r="G31" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E31/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F31)</f>
         <v>24102.039252927083</v>
       </c>
@@ -16311,7 +16310,7 @@
       <c r="F32" s="17">
         <v>10027</v>
       </c>
-      <c r="G32" s="18">
+      <c r="G32" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E32/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F32)</f>
         <v>28682.207125140892</v>
       </c>
@@ -16347,7 +16346,7 @@
       <c r="F33" s="17">
         <v>24062</v>
       </c>
-      <c r="G33" s="18">
+      <c r="G33" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E33/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F33)</f>
         <v>24729.3551597552</v>
       </c>
@@ -16383,7 +16382,7 @@
       <c r="F34" s="17">
         <v>54165</v>
       </c>
-      <c r="G34" s="18">
+      <c r="G34" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E34/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F34)</f>
         <v>24756.779887467252</v>
       </c>
@@ -16419,7 +16418,7 @@
       <c r="F35" s="17">
         <v>29456</v>
       </c>
-      <c r="G35" s="18">
+      <c r="G35" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E35/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F35)</f>
         <v>38131.272073997941</v>
       </c>
@@ -16455,7 +16454,7 @@
       <c r="F36" s="17">
         <v>51940</v>
       </c>
-      <c r="G36" s="18">
+      <c r="G36" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E36/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F36)</f>
         <v>39522.172573229953</v>
       </c>
@@ -16491,7 +16490,7 @@
       <c r="F37" s="17">
         <v>26216</v>
       </c>
-      <c r="G37" s="18">
+      <c r="G37" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E37/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F37)</f>
         <v>41149.315049000666</v>
       </c>
@@ -16527,7 +16526,7 @@
       <c r="F38" s="17">
         <v>19116</v>
       </c>
-      <c r="G38" s="18">
+      <c r="G38" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E38/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F38)</f>
         <v>34721.440603672949</v>
       </c>
@@ -16563,7 +16562,7 @@
       <c r="F39" s="17">
         <v>103050</v>
       </c>
-      <c r="G39" s="18">
+      <c r="G39" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E39/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F39)</f>
         <v>62024.058003517348</v>
       </c>
@@ -16599,7 +16598,7 @@
       <c r="F40" s="17">
         <v>70492</v>
       </c>
-      <c r="G40" s="18">
+      <c r="G40" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E40/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F40)</f>
         <v>87030.357806152431</v>
       </c>
@@ -16635,7 +16634,7 @@
       <c r="F41" s="17">
         <v>40494</v>
       </c>
-      <c r="G41" s="18">
+      <c r="G41" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E41/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F41)</f>
         <v>46584.773505120465</v>
       </c>
@@ -16671,7 +16670,7 @@
       <c r="F42" s="17">
         <v>71665</v>
       </c>
-      <c r="G42" s="18">
+      <c r="G42" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E42/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F42)</f>
         <v>47604.683886873958</v>
       </c>
@@ -16707,7 +16706,7 @@
       <c r="F43" s="17">
         <v>33751</v>
       </c>
-      <c r="G43" s="18">
+      <c r="G43" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E43/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F43)</f>
         <v>32495.972476580944</v>
       </c>
@@ -16743,7 +16742,7 @@
       <c r="F44" s="17">
         <v>15923</v>
       </c>
-      <c r="G44" s="18">
+      <c r="G44" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E44/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F44)</f>
         <v>31477.897981871723</v>
       </c>
@@ -16779,7 +16778,7 @@
       <c r="F45" s="17">
         <v>14401</v>
       </c>
-      <c r="G45" s="18">
+      <c r="G45" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E45/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F45)</f>
         <v>30299.477232605408</v>
       </c>
@@ -16815,7 +16814,7 @@
       <c r="F46" s="17">
         <v>21186</v>
       </c>
-      <c r="G46" s="18">
+      <c r="G46" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E46/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F46)</f>
         <v>33787.587629650239</v>
       </c>
@@ -16851,7 +16850,7 @@
       <c r="F47" s="17">
         <v>18628</v>
       </c>
-      <c r="G47" s="18">
+      <c r="G47" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E47/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F47)</f>
         <v>39102.811980679857</v>
       </c>
@@ -16887,7 +16886,7 @@
       <c r="F48" s="17">
         <v>105481</v>
       </c>
-      <c r="G48" s="18">
+      <c r="G48" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E48/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F48)</f>
         <v>132068.37499171778</v>
       </c>
@@ -16923,7 +16922,7 @@
       <c r="F49" s="17">
         <v>28795</v>
       </c>
-      <c r="G49" s="18">
+      <c r="G49" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E49/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F49)</f>
         <v>79680.996578228165</v>
       </c>
@@ -16959,7 +16958,7 @@
       <c r="F50" s="17">
         <v>67881</v>
       </c>
-      <c r="G50" s="18">
+      <c r="G50" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E50/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F50)</f>
         <v>80252.991355775404</v>
       </c>
@@ -16995,7 +16994,7 @@
       <c r="F51" s="17">
         <v>43628</v>
       </c>
-      <c r="G51" s="18">
+      <c r="G51" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E51/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F51)</f>
         <v>22133.021034030244</v>
       </c>
@@ -17031,7 +17030,7 @@
       <c r="F52" s="17">
         <v>35114</v>
       </c>
-      <c r="G52" s="18">
+      <c r="G52" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E52/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F52)</f>
         <v>69110.635130993978</v>
       </c>
@@ -17067,7 +17066,7 @@
       <c r="F53" s="17">
         <v>34794</v>
       </c>
-      <c r="G53" s="18">
+      <c r="G53" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E53/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F53)</f>
         <v>21186.342526283948</v>
       </c>
@@ -17103,7 +17102,7 @@
       <c r="F54" s="17">
         <v>17559</v>
       </c>
-      <c r="G54" s="18">
+      <c r="G54" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E54/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F54)</f>
         <v>39469.340982819718</v>
       </c>
@@ -17139,7 +17138,7 @@
       <c r="F55" s="17">
         <v>38303</v>
       </c>
-      <c r="G55" s="18">
+      <c r="G55" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E55/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F55)</f>
         <v>47154.419146919623</v>
       </c>
@@ -17175,7 +17174,7 @@
       <c r="F56" s="17">
         <v>13418</v>
       </c>
-      <c r="G56" s="18">
+      <c r="G56" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E56/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F56)</f>
         <v>57214.702043108235</v>
       </c>
@@ -17211,7 +17210,7 @@
       <c r="F57" s="17">
         <v>6799</v>
       </c>
-      <c r="G57" s="18">
+      <c r="G57" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E57/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F57)</f>
         <v>26076.45082477948</v>
       </c>
@@ -17247,7 +17246,7 @@
       <c r="F58" s="17">
         <v>63020</v>
       </c>
-      <c r="G58" s="18">
+      <c r="G58" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E58/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F58)</f>
         <v>35214.136521761393</v>
       </c>
@@ -17283,7 +17282,7 @@
       <c r="F59" s="17">
         <v>6820</v>
       </c>
-      <c r="G59" s="18">
+      <c r="G59" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E59/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F59)</f>
         <v>32501.621393301077</v>
       </c>
@@ -17319,7 +17318,7 @@
       <c r="F60" s="17">
         <v>7262</v>
       </c>
-      <c r="G60" s="18">
+      <c r="G60" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E60/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F60)</f>
         <v>15798.065563948701</v>
       </c>
@@ -17355,7 +17354,7 @@
       <c r="F61" s="17">
         <v>55628</v>
       </c>
-      <c r="G61" s="18">
+      <c r="G61" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E61/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F61)</f>
         <v>28099.521142193684</v>
       </c>
@@ -17391,7 +17390,7 @@
       <c r="F62" s="17">
         <v>38816</v>
       </c>
-      <c r="G62" s="18">
+      <c r="G62" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E62/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F62)</f>
         <v>22706.226388604227</v>
       </c>
@@ -17427,7 +17426,7 @@
       <c r="F63" s="17">
         <v>27300</v>
       </c>
-      <c r="G63" s="18">
+      <c r="G63" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E63/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F63)</f>
         <v>22341.588164472676</v>
       </c>
@@ -17463,7 +17462,7 @@
       <c r="F64" s="17">
         <v>14105</v>
       </c>
-      <c r="G64" s="18">
+      <c r="G64" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E64/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F64)</f>
         <v>27167.916646258567</v>
       </c>
@@ -17499,7 +17498,7 @@
       <c r="F65" s="17">
         <v>71399</v>
       </c>
-      <c r="G65" s="18">
+      <c r="G65" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E65/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F65)</f>
         <v>18843.410762878077</v>
       </c>
@@ -17535,7 +17534,7 @@
       <c r="F66" s="17">
         <v>53971</v>
       </c>
-      <c r="G66" s="18">
+      <c r="G66" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E66/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F66)</f>
         <v>23322.348221095031</v>
       </c>
@@ -17571,7 +17570,7 @@
       <c r="F67" s="17">
         <v>42298</v>
       </c>
-      <c r="G67" s="18">
+      <c r="G67" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E67/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F67)</f>
         <v>223802.56603653272</v>
       </c>
@@ -17607,7 +17606,7 @@
       <c r="F68" s="17">
         <v>57182</v>
       </c>
-      <c r="G68" s="18">
+      <c r="G68" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E68/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F68)</f>
         <v>39726.370235401198</v>
       </c>
@@ -17643,7 +17642,7 @@
       <c r="F69" s="17">
         <v>25065</v>
       </c>
-      <c r="G69" s="18">
+      <c r="G69" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E69/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F69)</f>
         <v>25858.934477835541</v>
       </c>
@@ -17679,7 +17678,7 @@
       <c r="F70" s="17">
         <v>12707</v>
       </c>
-      <c r="G70" s="18">
+      <c r="G70" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E70/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F70)</f>
         <v>21337.374237883843</v>
       </c>
@@ -17715,7 +17714,7 @@
       <c r="F71" s="17">
         <v>18394</v>
       </c>
-      <c r="G71" s="18">
+      <c r="G71" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E71/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F71)</f>
         <v>25897.457257597245</v>
       </c>
@@ -17751,7 +17750,7 @@
       <c r="F72" s="17">
         <v>29647</v>
       </c>
-      <c r="G72" s="18">
+      <c r="G72" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E72/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F72)</f>
         <v>19433.487034025991</v>
       </c>
@@ -17787,7 +17786,7 @@
       <c r="F73" s="17">
         <v>17433</v>
       </c>
-      <c r="G73" s="18">
+      <c r="G73" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E73/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F73)</f>
         <v>21817.113762547422</v>
       </c>
@@ -17823,7 +17822,7 @@
       <c r="F74" s="17">
         <v>33662</v>
       </c>
-      <c r="G74" s="18">
+      <c r="G74" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E74/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F74)</f>
         <v>25785.84819984468</v>
       </c>
@@ -17859,7 +17858,7 @@
       <c r="F75" s="17">
         <v>26104</v>
       </c>
-      <c r="G75" s="18">
+      <c r="G75" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E75/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F75)</f>
         <v>22181.714648980716</v>
       </c>
@@ -17895,7 +17894,7 @@
       <c r="F76" s="17">
         <v>77122</v>
       </c>
-      <c r="G76" s="18">
+      <c r="G76" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E76/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F76)</f>
         <v>29475.707213328249</v>
       </c>
@@ -17931,7 +17930,7 @@
       <c r="F77" s="17">
         <v>87781</v>
       </c>
-      <c r="G77" s="18">
+      <c r="G77" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E77/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F77)</f>
         <v>59225.637834689638</v>
       </c>
@@ -17967,7 +17966,7 @@
       <c r="F78" s="17">
         <v>24425</v>
       </c>
-      <c r="G78" s="18">
+      <c r="G78" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E78/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F78)</f>
         <v>23318.122846135077</v>
       </c>
@@ -17993,9 +17992,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -18038,16 +18039,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <f>FACTORS_MUNI!G1</f>
-        <v>PCT_EDA_POP</v>
-      </c>
-      <c r="B5" s="2">
-        <v>-1</v>
-      </c>
-    </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="colorScale" priority="4">
       <colorScale>
@@ -18059,9 +18054,6 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>